<commit_message>
Cambi vari: tolti cambi alle ricerche locali, uniformati euristici nel nuovo tentativo di gestire commesse identiche, test di interfaccia, messo un po' a posto il discorso parametri + GRASP
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_input/vettori.xlsx
+++ b/PS-VRP/Dati_input/vettori.xlsx
@@ -1,22 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frenc\Documents\GitHub\progettoIS\PS-VRP\Dati_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702D4CB8-58BC-4C91-9392-1FE01DCA9F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC77B75E-71BA-4D9F-934D-41D9F6367DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9135" yWindow="2490" windowWidth="16665" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={6E188874-A8F9-49FC-B9D3-68C66D740B1B}</author>
+  </authors>
+  <commentList>
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{6E188874-A8F9-49FC-B9D3-68C66D740B1B}">
+      <text>
+        <t>[Commento in thread]
+La versione di Excel in uso consente di leggere questo commento in thread, ma tutte le modifiche a esso apportate verranno rimosse se il file viene aperto in una versione più recente di Excel. Ulteriori informazioni: https://go.microsoft.com/fwlink/?linkid=870924
+Commento:
+Aggiunto in post - è come dovrebbe essere, non com’era</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -41,7 +59,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -56,6 +74,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,6 +128,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="FRANCESCO MERCALLI" id="{1AAB30E2-AD09-41A1-B033-C5E2EB1653E7}" userId="S::309705@unimore.it::6547cca3-b3bb-452c-8ca4-97fb14c1fe06" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -421,12 +451,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A5" dT="2025-09-03T16:25:10.32" personId="{1AAB30E2-AD09-41A1-B033-C5E2EB1653E7}" id="{6E188874-A8F9-49FC-B9D3-68C66D740B1B}">
+    <text>Aggiunto in post - è come dovrebbe essere, non com’era</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -487,7 +525,19 @@
         <v>14680</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>40032</v>
+      </c>
+      <c r="B5" s="3">
+        <v>45848</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
PROVA - implementate, al meglio delle mie possibilità, le nuove logiche di ricerca locale; convalidati i calcoli riguardo la capacità e il ragionamento generale; cambiati i pesi delle ricerche locali
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_input/vettori.xlsx
+++ b/PS-VRP/Dati_input/vettori.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alecola\Desktop\PS-VRP\Dati_input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frenc\Documents\GitHub\progettoIS\PS-VRP\Dati_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C2F06F-A99F-46B2-AB0D-AC6DB5210C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65549AAE-C80C-4ABC-86C5-3056CFDC3981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="3192" windowWidth="18840" windowHeight="10632" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5790" yWindow="3255" windowWidth="16665" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="dd\-mm\-yyyy"/>
+    <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -58,12 +58,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -78,7 +90,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -86,7 +98,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -423,15 +450,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.21875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -445,7 +472,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>40299</v>
       </c>
@@ -459,7 +486,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>40294</v>
       </c>
@@ -473,7 +500,7 @@
         <v>11395.8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>40306</v>
       </c>
@@ -487,7 +514,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>40290</v>
       </c>
@@ -501,7 +528,7 @@
         <v>6638.46</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>40305</v>
       </c>
@@ -515,7 +542,7 @@
         <v>4950.96</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>40274</v>
       </c>
@@ -523,7 +550,7 @@
         <v>45912</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>40289</v>
       </c>
@@ -531,7 +558,7 @@
         <v>45910</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>40295</v>
       </c>
@@ -543,6 +570,104 @@
       </c>
       <c r="D9" s="2">
         <v>4846</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>40279</v>
+      </c>
+      <c r="B10" s="5">
+        <v>45910</v>
+      </c>
+      <c r="C10" s="6">
+        <v>5</v>
+      </c>
+      <c r="D10" s="4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>40900</v>
+      </c>
+      <c r="B11" s="8">
+        <v>45921</v>
+      </c>
+      <c r="C11" s="7">
+        <v>2</v>
+      </c>
+      <c r="D11" s="7">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>40902</v>
+      </c>
+      <c r="B12" s="8">
+        <v>45923</v>
+      </c>
+      <c r="C12" s="7">
+        <v>12</v>
+      </c>
+      <c r="D12" s="7">
+        <v>10002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>40904</v>
+      </c>
+      <c r="B13" s="8">
+        <v>45925</v>
+      </c>
+      <c r="C13" s="7">
+        <v>4</v>
+      </c>
+      <c r="D13" s="7">
+        <v>10004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>40905</v>
+      </c>
+      <c r="B14" s="8">
+        <v>45926</v>
+      </c>
+      <c r="C14" s="7">
+        <v>12</v>
+      </c>
+      <c r="D14" s="7">
+        <v>10005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>40910</v>
+      </c>
+      <c r="B15" s="8">
+        <v>45921</v>
+      </c>
+      <c r="C15" s="7">
+        <v>6</v>
+      </c>
+      <c r="D15" s="7">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>40911</v>
+      </c>
+      <c r="B16" s="8">
+        <v>45921</v>
+      </c>
+      <c r="C16" s="7">
+        <v>5</v>
+      </c>
+      <c r="D16" s="7">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PROVA - implementati tutti i cambiamenti; rivedere eventualmente logica dei ritardi con tempo medio applicata indiscriminatamente a tutte le commesse zona chiusa
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_input/vettori.xlsx
+++ b/PS-VRP/Dati_input/vettori.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frenc\Documents\GitHub\progettoIS\PS-VRP\Dati_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65549AAE-C80C-4ABC-86C5-3056CFDC3981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AF5162-A344-4438-9634-AB666BA38D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5790" yWindow="3255" windowWidth="16665" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="16665" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
+    <numFmt numFmtId="166" formatCode="dd\-mm\-yyyy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -58,7 +58,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -67,13 +67,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -90,7 +84,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -98,24 +92,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -450,13 +436,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="21.7109375" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -474,200 +460,252 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>40299</v>
+        <v>40606</v>
       </c>
       <c r="B2" s="3">
-        <v>45908</v>
+        <v>45975</v>
       </c>
       <c r="C2" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2">
-        <v>9000</v>
+        <v>8165</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>40294</v>
+        <v>40655</v>
       </c>
       <c r="B3" s="3">
-        <v>45904</v>
+        <v>45974</v>
       </c>
       <c r="C3" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D3" s="2">
-        <v>11395.8</v>
+        <v>4491.5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>40306</v>
+        <v>40642</v>
       </c>
       <c r="B4" s="3">
-        <v>45905</v>
+        <v>45975</v>
       </c>
       <c r="C4" s="2">
         <v>6</v>
       </c>
       <c r="D4" s="2">
-        <v>6000</v>
+        <v>4850</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>40290</v>
+        <v>40624</v>
       </c>
       <c r="B5" s="3">
-        <v>45908</v>
+        <v>45980</v>
       </c>
       <c r="C5" s="2">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D5" s="2">
-        <v>6638.46</v>
+        <v>597.85</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>40305</v>
+        <v>40652</v>
       </c>
       <c r="B6" s="3">
-        <v>45904</v>
-      </c>
-      <c r="C6" s="2">
-        <v>2</v>
-      </c>
-      <c r="D6" s="2">
-        <v>4950.96</v>
+        <v>45992</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>40274</v>
+        <v>40649</v>
       </c>
       <c r="B7" s="3">
-        <v>45912</v>
+        <v>45980</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>40289</v>
+        <v>40628</v>
       </c>
       <c r="B8" s="3">
-        <v>45910</v>
+        <v>45978</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>40295</v>
+        <v>40627</v>
       </c>
       <c r="B9" s="3">
-        <v>45908</v>
-      </c>
-      <c r="C9" s="2">
+        <v>45975</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>40623</v>
+      </c>
+      <c r="B10" s="3">
+        <v>45974</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>5544.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>40637</v>
+      </c>
+      <c r="B11" s="3">
+        <v>45973</v>
+      </c>
+      <c r="C11" s="2">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2">
+        <v>6489.82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>406062</v>
+      </c>
+      <c r="B12" s="5">
+        <v>45982</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4">
+        <v>8165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>406552</v>
+      </c>
+      <c r="B13" s="5">
+        <v>45981</v>
+      </c>
+      <c r="C13" s="4">
+        <v>4</v>
+      </c>
+      <c r="D13" s="4">
+        <v>4491.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>406422</v>
+      </c>
+      <c r="B14" s="5">
+        <v>45982</v>
+      </c>
+      <c r="C14" s="4">
+        <v>6</v>
+      </c>
+      <c r="D14" s="4">
+        <v>4850</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>406242</v>
+      </c>
+      <c r="B15" s="5">
+        <v>45987</v>
+      </c>
+      <c r="C15" s="4">
         <v>5</v>
       </c>
-      <c r="D9" s="2">
-        <v>4846</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>40279</v>
-      </c>
-      <c r="B10" s="5">
-        <v>45910</v>
-      </c>
-      <c r="C10" s="6">
-        <v>5</v>
-      </c>
-      <c r="D10" s="4">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
-        <v>40900</v>
-      </c>
-      <c r="B11" s="8">
-        <v>45921</v>
-      </c>
-      <c r="C11" s="7">
+      <c r="D15" s="4">
+        <v>597.85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>406522</v>
+      </c>
+      <c r="B16" s="5">
+        <v>45999</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>406492</v>
+      </c>
+      <c r="B17" s="5">
+        <v>45987</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>406282</v>
+      </c>
+      <c r="B18" s="5">
+        <v>45985</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>406272</v>
+      </c>
+      <c r="B19" s="5">
+        <v>45982</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>406232</v>
+      </c>
+      <c r="B20" s="5">
+        <v>45981</v>
+      </c>
+      <c r="C20" s="4">
         <v>2</v>
       </c>
-      <c r="D11" s="7">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
-        <v>40902</v>
-      </c>
-      <c r="B12" s="8">
-        <v>45923</v>
-      </c>
-      <c r="C12" s="7">
-        <v>12</v>
-      </c>
-      <c r="D12" s="7">
-        <v>10002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
-        <v>40904</v>
-      </c>
-      <c r="B13" s="8">
-        <v>45925</v>
-      </c>
-      <c r="C13" s="7">
+      <c r="D20" s="4">
+        <v>5544.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>406372</v>
+      </c>
+      <c r="B21" s="5">
+        <v>45980</v>
+      </c>
+      <c r="C21" s="4">
         <v>4</v>
       </c>
-      <c r="D13" s="7">
-        <v>10004</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
-        <v>40905</v>
-      </c>
-      <c r="B14" s="8">
-        <v>45926</v>
-      </c>
-      <c r="C14" s="7">
-        <v>12</v>
-      </c>
-      <c r="D14" s="7">
-        <v>10005</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
-        <v>40910</v>
-      </c>
-      <c r="B15" s="8">
-        <v>45921</v>
-      </c>
-      <c r="C15" s="7">
-        <v>6</v>
-      </c>
-      <c r="D15" s="7">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
-        <v>40911</v>
-      </c>
-      <c r="B16" s="8">
-        <v>45921</v>
-      </c>
-      <c r="C16" s="7">
-        <v>5</v>
-      </c>
-      <c r="D16" s="7">
-        <v>10000</v>
+      <c r="D21" s="4">
+        <v>6489.82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>